<commit_message>
graphs for income dist, spending ratio and living area protection increase
</commit_message>
<xml_diff>
--- a/Scripts_annehuitema2003/Copy exel - graphs/Copy_data_ouput_exceladjustments/Copy_Income_dist_housinggame_session_20_251007_VerzekeraarsMasterClass.xlsx
+++ b/Scripts_annehuitema2003/Copy exel - graphs/Copy_data_ouput_exceladjustments/Copy_Income_dist_housinggame_session_20_251007_VerzekeraarsMasterClass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a040831fc7e8278/Bureaublad/BEP/Copy_data_ouput_exceladjustments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1a040831fc7e8278/Bureaublad/BEP data analysis/Scripts_annehuitema2003/Copy exel - graphs/Copy_data_ouput_exceladjustments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="869" documentId="8_{19952296-3D70-421E-BC6F-4638A080F461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDB66B88-E622-43AE-879E-801A479B0A45}"/>
+  <xr:revisionPtr revIDLastSave="876" documentId="8_{19952296-3D70-421E-BC6F-4638A080F461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CEF64D6-0356-41CA-8888-B8BCF63C0659}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="df_income_dist" sheetId="1" r:id="rId1"/>
@@ -27,10 +27,10 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId12"/>
-    <pivotCache cacheId="10" r:id="rId13"/>
-    <pivotCache cacheId="15" r:id="rId14"/>
-    <pivotCache cacheId="56" r:id="rId15"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="2" r:id="rId14"/>
+    <pivotCache cacheId="3" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="173">
   <si>
     <t>playerround_id</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t xml:space="preserve">Gemiddelde van Added_total_damage </t>
+  </si>
+  <si>
+    <t>(Meerdere items)</t>
   </si>
 </sst>
 </file>
@@ -1942,6 +1945,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1998,6 +2004,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2054,6 +2063,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2110,6 +2122,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2166,6 +2181,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2222,6 +2240,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2278,6 +2299,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2614,6 +2638,9 @@
       <c:pivotFmt>
         <c:idx val="12"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2641,6 +2668,9 @@
       <c:pivotFmt>
         <c:idx val="13"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2654,6 +2684,62 @@
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4722,6 +4808,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="416584640"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4913,19 +5000,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -4981,19 +5056,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5049,19 +5112,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5132,19 +5183,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5200,19 +5239,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -5733,19 +5760,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -6006,13 +6021,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>6337.5</c:v>
+                  <c:v>2620</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2531.25</c:v>
+                  <c:v>1166.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>500</c:v>
+                  <c:v>1035</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -6089,22 +6104,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7250</c:v>
+                  <c:v>5650</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9750</c:v>
+                  <c:v>7800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9500</c:v>
+                  <c:v>8050</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15625</c:v>
+                  <c:v>12500</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15625</c:v>
+                  <c:v>12500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24000</c:v>
+                  <c:v>17700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6175,19 +6190,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17500</c:v>
+                  <c:v>6500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31250</c:v>
+                  <c:v>6250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6255,22 +6270,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6338,22 +6353,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9000</c:v>
+                  <c:v>2650</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>500</c:v>
+                  <c:v>3350</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9500</c:v>
+                  <c:v>4250</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6550</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5500</c:v>
+                  <c:v>7200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6421,22 +6436,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3525</c:v>
+                  <c:v>1632.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4625</c:v>
+                  <c:v>2933.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10312.5</c:v>
+                  <c:v>4517.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14393.75</c:v>
+                  <c:v>8023.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19718.75</c:v>
+                  <c:v>13237.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30768.75</c:v>
+                  <c:v>18183.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6540,22 +6555,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.75</c:v>
+                  <c:v>6.45</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.25</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.5</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.75</c:v>
+                  <c:v>10.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6688,6 +6703,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="398809792"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
@@ -6790,6 +6806,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="398808832"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -6904,6 +6921,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="742620480"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -7930,6 +7948,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="753832384"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -10980,10 +10999,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Anne Sophia Huitema" refreshedDate="45986.711180439816" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="120" xr:uid="{96F1B8EE-F2BB-4EF9-92E3-E4FD9B5FE085}">
   <cacheSource type="worksheet">
@@ -57954,7 +57969,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60FFC6A6-2085-4B2B-91B4-5DAB3F981487}" name="Draaitabel5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{60FFC6A6-2085-4B2B-91B4-5DAB3F981487}" name="Draaitabel5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:H8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -58121,7 +58136,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2F9DC0F4-5597-4145-9B41-B93D95B9AB1A}" name="Draaitabel1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2F9DC0F4-5597-4145-9B41-B93D95B9AB1A}" name="Draaitabel1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A3:H10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="31">
     <pivotField dataField="1" showAll="0"/>
@@ -58230,7 +58245,7 @@
   <dataFields count="1">
     <dataField name="Som van satisfaction_total" fld="0" baseField="23" baseItem="0"/>
   </dataFields>
-  <chartFormats count="14">
+  <chartFormats count="15">
     <chartFormat chart="3" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -58396,6 +58411,18 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="3" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="30" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -58410,7 +58437,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1805EEEB-EE43-4EC8-A064-B81480BB1276}" name="Draaitabel2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1805EEEB-EE43-4EC8-A064-B81480BB1276}" name="Draaitabel2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A3:D10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="54">
     <pivotField showAll="0"/>
@@ -58747,7 +58774,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD1C762E-AE67-4EBE-AF75-9A6259A790D8}" name="Draaitabel5" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AD1C762E-AE67-4EBE-AF75-9A6259A790D8}" name="Draaitabel5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="A3:H10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="55">
     <pivotField showAll="0"/>
@@ -58796,10 +58823,10 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="7">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
         <item x="4"/>
         <item h="1" x="5"/>
         <item t="default"/>
@@ -58819,8 +58846,8 @@
         <item x="1"/>
         <item x="4"/>
         <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -58980,7 +59007,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3FFC3C5D-1EBA-43B1-B5AE-A7EE39838B5D}" name="Draaitabel13" cacheId="56" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3FFC3C5D-1EBA-43B1-B5AE-A7EE39838B5D}" name="Draaitabel13" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:D10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="55">
     <pivotField showAll="0"/>
@@ -66612,7 +66639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B30CAEA-ED29-483A-9819-2678604F83CE}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="95" workbookViewId="0">
+    <sheetView topLeftCell="B31" zoomScale="95" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -66651,13 +66678,13 @@
       <c r="A4" s="5">
         <v>123</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4">
         <v>2650</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4">
         <v>2400</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -66665,13 +66692,13 @@
       <c r="A5" s="5">
         <v>124</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>3350</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5">
         <v>1600</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>5.5</v>
       </c>
     </row>
@@ -66679,13 +66706,13 @@
       <c r="A6" s="5">
         <v>125</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>4250</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>1200</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>6.45</v>
       </c>
     </row>
@@ -66693,13 +66720,13 @@
       <c r="A7" s="5">
         <v>126</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>5600</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <v>600</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>9.5</v>
       </c>
     </row>
@@ -66707,13 +66734,13 @@
       <c r="A8" s="5">
         <v>127</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>6550</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8">
         <v>400</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>10.25</v>
       </c>
     </row>
@@ -66721,13 +66748,13 @@
       <c r="A9" s="5">
         <v>128</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>7200</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>600</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>10.7</v>
       </c>
     </row>
@@ -66735,13 +66762,13 @@
       <c r="A10" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>4933.333333333333</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10">
         <v>1133.3333333333333</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>7.4333333333333336</v>
       </c>
     </row>
@@ -66755,8 +66782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BC314"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BC123" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="AT1" zoomScale="62" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AZ2" sqref="AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -89356,25 +89383,25 @@
       <c r="A5" s="5">
         <v>0</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>20</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5">
         <v>20</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>20</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5">
         <v>20</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5">
         <v>20</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5">
         <v>20</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5">
         <v>120</v>
       </c>
     </row>
@@ -89382,25 +89409,25 @@
       <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>19</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>18</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6">
         <v>27</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6">
         <v>21</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6">
         <v>26</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6">
         <v>123</v>
       </c>
     </row>
@@ -89408,25 +89435,25 @@
       <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <v>21</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>23</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7">
         <v>35</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7">
         <v>36</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7">
         <v>40</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7">
         <v>163</v>
       </c>
     </row>
@@ -89434,25 +89461,25 @@
       <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8">
         <v>20</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>25</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8">
         <v>47</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8">
         <v>54</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8">
         <v>53</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8">
         <v>202</v>
       </c>
     </row>
@@ -89460,25 +89487,25 @@
       <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>30</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>43</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9">
         <v>61</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9">
         <v>74</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9">
         <v>75</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9">
         <v>284</v>
       </c>
     </row>
@@ -89486,25 +89513,25 @@
       <c r="A10" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>44</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10">
         <v>110</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>129</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10">
         <v>190</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10">
         <v>205</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10">
         <v>214</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10">
         <v>892</v>
       </c>
     </row>
@@ -89571,13 +89598,13 @@
       <c r="A4" s="5">
         <v>123</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4">
         <v>9000</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4">
         <v>3525</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4">
         <v>0.25</v>
       </c>
     </row>
@@ -89585,13 +89612,13 @@
       <c r="A5" s="5">
         <v>124</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>500</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5">
         <v>4625</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5">
         <v>7.5</v>
       </c>
     </row>
@@ -89599,13 +89626,13 @@
       <c r="A6" s="5">
         <v>125</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>9500</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>10312.5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6">
         <v>10.75</v>
       </c>
     </row>
@@ -89613,13 +89640,13 @@
       <c r="A7" s="5">
         <v>126</v>
       </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>14393.75</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7">
         <v>15.25</v>
       </c>
     </row>
@@ -89627,13 +89654,13 @@
       <c r="A8" s="5">
         <v>127</v>
       </c>
-      <c r="B8" s="6">
-        <v>0</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>19718.75</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8">
         <v>18.5</v>
       </c>
     </row>
@@ -89641,13 +89668,13 @@
       <c r="A9" s="5">
         <v>128</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9">
         <v>5500</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9">
         <v>30768.75</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9">
         <v>18.75</v>
       </c>
     </row>
@@ -89655,13 +89682,13 @@
       <c r="A10" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>4083.3333333333335</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10">
         <v>13890.625</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10">
         <v>11.833333333333334</v>
       </c>
     </row>
@@ -89678,20 +89705,20 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" zoomScale="61" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="67" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.77734375" bestFit="1" customWidth="1"/>
@@ -89725,8 +89752,8 @@
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5">
-        <v>4</v>
+      <c r="B1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -89760,25 +89787,25 @@
         <v>123</v>
       </c>
       <c r="B4" s="6">
-        <v>6337.5</v>
+        <v>2620</v>
       </c>
       <c r="C4" s="6">
-        <v>7250</v>
+        <v>5650</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>2000</v>
+        <v>2400</v>
       </c>
       <c r="F4" s="6">
-        <v>9000</v>
+        <v>2650</v>
       </c>
       <c r="G4" s="6">
-        <v>3525</v>
+        <v>1632.5</v>
       </c>
       <c r="H4" s="6">
-        <v>0.25</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -89786,25 +89813,25 @@
         <v>124</v>
       </c>
       <c r="B5" s="6">
-        <v>2531.25</v>
+        <v>1166.25</v>
       </c>
       <c r="C5" s="6">
-        <v>9750</v>
+        <v>7800</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="E5" s="6">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="F5" s="6">
-        <v>500</v>
+        <v>3350</v>
       </c>
       <c r="G5" s="6">
-        <v>4625</v>
+        <v>2933.75</v>
       </c>
       <c r="H5" s="6">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -89812,25 +89839,25 @@
         <v>125</v>
       </c>
       <c r="B6" s="6">
-        <v>500</v>
+        <v>1035</v>
       </c>
       <c r="C6" s="6">
-        <v>9500</v>
+        <v>8050</v>
       </c>
       <c r="D6" s="6">
-        <v>17500</v>
+        <v>6500</v>
       </c>
       <c r="E6" s="6">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="F6" s="6">
-        <v>9500</v>
+        <v>4250</v>
       </c>
       <c r="G6" s="6">
-        <v>10312.5</v>
+        <v>4517.5</v>
       </c>
       <c r="H6" s="6">
-        <v>10.75</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -89841,22 +89868,22 @@
         <v>0</v>
       </c>
       <c r="C7" s="6">
-        <v>15625</v>
+        <v>12500</v>
       </c>
       <c r="D7" s="6">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="E7" s="6">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F7" s="6">
-        <v>0</v>
+        <v>5600</v>
       </c>
       <c r="G7" s="6">
-        <v>14393.75</v>
+        <v>8023.75</v>
       </c>
       <c r="H7" s="6">
-        <v>15.25</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -89867,22 +89894,22 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>15625</v>
+        <v>12500</v>
       </c>
       <c r="D8" s="6">
         <v>0</v>
       </c>
       <c r="E8" s="6">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="F8" s="6">
-        <v>0</v>
+        <v>6550</v>
       </c>
       <c r="G8" s="6">
-        <v>19718.75</v>
+        <v>13237.5</v>
       </c>
       <c r="H8" s="6">
-        <v>18.5</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -89893,22 +89920,22 @@
         <v>0</v>
       </c>
       <c r="C9" s="6">
-        <v>24000</v>
+        <v>17700</v>
       </c>
       <c r="D9" s="6">
-        <v>31250</v>
+        <v>6250</v>
       </c>
       <c r="E9" s="6">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F9" s="6">
-        <v>5500</v>
+        <v>7200</v>
       </c>
       <c r="G9" s="6">
-        <v>30768.75</v>
+        <v>18183.75</v>
       </c>
       <c r="H9" s="6">
-        <v>18.75</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -89916,25 +89943,25 @@
         <v>159</v>
       </c>
       <c r="B10" s="6">
-        <v>1561.4583333333333</v>
+        <v>803.54166666666663</v>
       </c>
       <c r="C10" s="6">
-        <v>13625</v>
+        <v>10700</v>
       </c>
       <c r="D10" s="6">
-        <v>8125</v>
+        <v>2750</v>
       </c>
       <c r="E10" s="6">
-        <v>666.66666666666663</v>
+        <v>1133.3333333333333</v>
       </c>
       <c r="F10" s="6">
-        <v>4083.3333333333335</v>
+        <v>4933.333333333333</v>
       </c>
       <c r="G10" s="6">
-        <v>13890.625</v>
+        <v>8088.125</v>
       </c>
       <c r="H10" s="6">
-        <v>11.833333333333334</v>
+        <v>7.4333333333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>